<commit_message>
Results from ranking decisions and computing rewards
</commit_message>
<xml_diff>
--- a/results/ranking/Correlations_CycleSimilarityMetrics.xlsx
+++ b/results/ranking/Correlations_CycleSimilarityMetrics.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chris\OneDrive\Documentos\GitHub\ML_SelfHealingUtility\data\Ranking\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Chris\Documents\GitHub\ML_SelfHealingUtility\results\ranking\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="18270" windowHeight="7530" xr2:uid="{BAB77291-47AC-4F74-8855-905206CB7EF3}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18270" windowHeight="7530" xr2:uid="{BAB77291-47AC-4F74-8855-905206CB7EF3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -56,10 +56,10 @@
     <t>Metric</t>
   </si>
   <si>
-    <t>Dataset size</t>
-  </si>
-  <si>
     <t>Cycle range</t>
+  </si>
+  <si>
+    <t>Trainind dataset size</t>
   </si>
 </sst>
 </file>
@@ -95,13 +95,45 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="7">
+    <dxf>
+      <alignment horizontal="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -115,32 +147,20 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B346DAA1-5164-4CEB-84D5-B9D1CC5F0D47}" name="Table1" displayName="Table1" ref="B2:H20" totalsRowShown="0">
-  <autoFilter ref="B2:H20" xr:uid="{69FA9D87-C040-46CF-BAE4-9976CC3CDE98}">
-    <filterColumn colId="0">
-      <filters>
-        <filter val="Up to 30"/>
-      </filters>
-    </filterColumn>
-    <filterColumn colId="5">
-      <filters>
-        <filter val="Jaccard"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
-  <sortState ref="B5:H20">
-    <sortCondition ref="H2:H20"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B346DAA1-5164-4CEB-84D5-B9D1CC5F0D47}" name="Table1" displayName="Table1" ref="B2:H20" totalsRowShown="0" headerRowDxfId="6">
+  <sortState ref="B3:H20">
+    <sortCondition ref="B2:B20"/>
   </sortState>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{DC50DEB0-D40B-42B0-98C8-0EB9219891EC}" name="Cycle range"/>
-    <tableColumn id="2" xr3:uid="{955E98C8-9EF1-446C-8F55-A3EBA46A1E11}" name="Linear"/>
-    <tableColumn id="3" xr3:uid="{DECFE54E-D3CA-44FD-9E53-1615B5FBAC76}" name="Discontinuous"/>
-    <tableColumn id="4" xr3:uid="{EE1A0DE0-F017-46C6-A67F-DD28AC24170F}" name="Saturating"/>
-    <tableColumn id="5" xr3:uid="{09294846-1A5F-4ED7-A270-28A8655F77A3}" name="Combined"/>
-    <tableColumn id="6" xr3:uid="{72F0401A-C3DF-44FA-88D1-8D3A2082844E}" name="Metric"/>
-    <tableColumn id="7" xr3:uid="{1116271A-AC81-4CC0-B423-36D0A0FCB010}" name="Dataset size"/>
+    <tableColumn id="1" xr3:uid="{DC50DEB0-D40B-42B0-98C8-0EB9219891EC}" name="Cycle range" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{955E98C8-9EF1-446C-8F55-A3EBA46A1E11}" name="Linear" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{DECFE54E-D3CA-44FD-9E53-1615B5FBAC76}" name="Discontinuous" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{EE1A0DE0-F017-46C6-A67F-DD28AC24170F}" name="Saturating" dataDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{09294846-1A5F-4ED7-A270-28A8655F77A3}" name="Combined" dataDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{72F0401A-C3DF-44FA-88D1-8D3A2082844E}" name="Metric" dataDxfId="2"/>
+    <tableColumn id="7" xr3:uid="{1116271A-AC81-4CC0-B423-36D0A0FCB010}" name="Trainind dataset size"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -444,448 +464,449 @@
   <dimension ref="B2:H20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="12.26953125" customWidth="1"/>
-    <col min="4" max="4" width="15.1796875" customWidth="1"/>
-    <col min="5" max="6" width="13.54296875" customWidth="1"/>
-    <col min="8" max="8" width="12.90625" customWidth="1"/>
+    <col min="2" max="2" width="12.265625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="15.19921875" customWidth="1"/>
+    <col min="5" max="6" width="13.53125" customWidth="1"/>
+    <col min="7" max="7" width="9.06640625" style="4"/>
+    <col min="8" max="8" width="13.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B2" t="s">
+    <row r="2" spans="2:8" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G2" t="s">
-        <v>9</v>
-      </c>
-      <c r="H2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="2:8" hidden="1" x14ac:dyDescent="0.35">
-      <c r="B3" t="s">
+    </row>
+    <row r="3" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="B3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="2">
         <v>-0.39005589454965633</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="2">
         <v>-0.86209320007329493</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="2">
         <v>-0.82122480591543989</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="2">
         <v>-0.89741626153717469</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" s="4" t="s">
         <v>8</v>
       </c>
       <c r="H3">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="2:8" hidden="1" x14ac:dyDescent="0.35">
-      <c r="B4" t="s">
+    <row r="4" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="B4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="2">
         <v>-0.36238802445372276</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="2">
         <v>-0.28268688093181399</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="2">
         <v>0.25241772205581392</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="2">
         <v>0.14679482417616607</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4" s="4" t="s">
         <v>7</v>
       </c>
       <c r="H4">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="2:8" hidden="1" x14ac:dyDescent="0.35">
-      <c r="B5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5">
-        <v>-0.13625781022048511</v>
-      </c>
-      <c r="D5">
-        <v>-0.45988451981245337</v>
-      </c>
-      <c r="E5">
-        <v>0.39582703496227761</v>
-      </c>
-      <c r="F5">
-        <v>0.21339957776542165</v>
-      </c>
-      <c r="G5" t="s">
-        <v>7</v>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="B5" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="2">
+        <v>-0.56786792831496236</v>
+      </c>
+      <c r="D5" s="2">
+        <v>-0.69372126001405321</v>
+      </c>
+      <c r="E5" s="2">
+        <v>-0.68417269470929032</v>
+      </c>
+      <c r="F5" s="2">
+        <v>-0.75612519234561926</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>0</v>
       </c>
       <c r="H5">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="2:8" hidden="1" x14ac:dyDescent="0.35">
-      <c r="B6" t="s">
+    <row r="6" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="B6" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C6">
-        <v>-0.56786792831496236</v>
-      </c>
-      <c r="D6">
-        <v>-0.69372126001405321</v>
-      </c>
-      <c r="E6">
-        <v>-0.68417269470929032</v>
-      </c>
-      <c r="F6">
-        <v>-0.75612519234561926</v>
-      </c>
-      <c r="G6" t="s">
+      <c r="C6" s="2">
+        <v>-0.29960088852974315</v>
+      </c>
+      <c r="D6" s="2">
+        <v>-0.9093991241335091</v>
+      </c>
+      <c r="E6" s="2">
+        <v>-0.90669507372884584</v>
+      </c>
+      <c r="F6" s="2">
+        <v>-0.87642903442130859</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="B7" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="2">
+        <v>-0.53246994822591609</v>
+      </c>
+      <c r="D7" s="2">
+        <v>-0.79359322745568095</v>
+      </c>
+      <c r="E7" s="2">
+        <v>-0.75392270877999112</v>
+      </c>
+      <c r="F7" s="2">
+        <v>-0.71018114887203065</v>
+      </c>
+      <c r="G7" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="H6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7">
-        <v>-0.44795076420059921</v>
-      </c>
-      <c r="D7">
-        <v>-0.86170020700246419</v>
-      </c>
-      <c r="E7">
-        <v>-0.44755059932294011</v>
-      </c>
-      <c r="F7">
-        <v>-0.64686361282490601</v>
-      </c>
-      <c r="G7" t="s">
-        <v>0</v>
-      </c>
       <c r="H7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="2:8" hidden="1" x14ac:dyDescent="0.35">
-      <c r="B8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="B8" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C8">
-        <v>-0.29960088852974315</v>
-      </c>
-      <c r="D8">
-        <v>-0.9093991241335091</v>
-      </c>
-      <c r="E8">
-        <v>-0.90669507372884584</v>
-      </c>
-      <c r="F8">
-        <v>-0.87642903442130859</v>
-      </c>
-      <c r="G8" t="s">
-        <v>8</v>
+      <c r="C8" s="2">
+        <v>-0.19103890278885322</v>
+      </c>
+      <c r="D8" s="2">
+        <v>-1.5624617602267566E-2</v>
+      </c>
+      <c r="E8" s="2">
+        <v>-0.57593386729312046</v>
+      </c>
+      <c r="F8" s="2">
+        <v>-3.1345402429609481E-2</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>7</v>
       </c>
       <c r="H8">
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="2:8" hidden="1" x14ac:dyDescent="0.35">
-      <c r="B9" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9">
-        <v>-0.48834910911226725</v>
-      </c>
-      <c r="D9">
-        <v>-0.92574421987418876</v>
-      </c>
-      <c r="E9">
-        <v>-0.55733843067043254</v>
-      </c>
-      <c r="F9">
-        <v>-0.67510037215646967</v>
-      </c>
-      <c r="G9" t="s">
+    <row r="9" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="B9" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="2">
+        <v>-0.46035458052708023</v>
+      </c>
+      <c r="D9" s="2">
+        <v>-0.8793866776678575</v>
+      </c>
+      <c r="E9" s="2">
+        <v>-0.80154448031778835</v>
+      </c>
+      <c r="F9" s="2">
+        <v>-0.8569551968436695</v>
+      </c>
+      <c r="G9" s="4" t="s">
         <v>8</v>
       </c>
       <c r="H9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="2:8" hidden="1" x14ac:dyDescent="0.35">
-      <c r="B10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="B10" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C10">
-        <v>-0.46035458052708023</v>
-      </c>
-      <c r="D10">
-        <v>-0.8793866776678575</v>
-      </c>
-      <c r="E10">
-        <v>-0.80154448031778835</v>
-      </c>
-      <c r="F10">
-        <v>-0.8569551968436695</v>
-      </c>
-      <c r="G10" t="s">
-        <v>8</v>
+      <c r="C10" s="2">
+        <v>-0.57230055083887155</v>
+      </c>
+      <c r="D10" s="2">
+        <v>-0.80095082363904357</v>
+      </c>
+      <c r="E10" s="2">
+        <v>-0.70901597017509299</v>
+      </c>
+      <c r="F10" s="2">
+        <v>-0.7387123142517128</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>0</v>
       </c>
       <c r="H10">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="2:8" hidden="1" x14ac:dyDescent="0.35">
-      <c r="B11" t="s">
+    <row r="11" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="B11" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" s="2">
+        <v>-0.36902571311328258</v>
+      </c>
+      <c r="D11" s="2">
+        <v>0.15981874291995243</v>
+      </c>
+      <c r="E11" s="2">
+        <v>-0.19843610814515833</v>
+      </c>
+      <c r="F11" s="2">
+        <v>7.6033443732449343E-2</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="H11">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="B12" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C11">
+      <c r="C12" s="2">
+        <v>-0.13625781022048511</v>
+      </c>
+      <c r="D12" s="2">
+        <v>-0.45988451981245337</v>
+      </c>
+      <c r="E12" s="2">
+        <v>0.39582703496227761</v>
+      </c>
+      <c r="F12" s="2">
+        <v>0.21339957776542165</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="H12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="B13" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" s="2">
+        <v>-0.44795076420059921</v>
+      </c>
+      <c r="D13" s="2">
+        <v>-0.86170020700246419</v>
+      </c>
+      <c r="E13" s="2">
+        <v>-0.44755059932294011</v>
+      </c>
+      <c r="F13" s="2">
+        <v>-0.64686361282490601</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="B14" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" s="2">
+        <v>-0.48834910911226725</v>
+      </c>
+      <c r="D14" s="2">
+        <v>-0.92574421987418876</v>
+      </c>
+      <c r="E14" s="2">
+        <v>-0.55733843067043254</v>
+      </c>
+      <c r="F14" s="2">
+        <v>-0.67510037215646967</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="B15" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" s="2">
         <v>-0.44078791706766474</v>
       </c>
-      <c r="D11">
+      <c r="D15" s="2">
         <v>-0.71782163823377798</v>
       </c>
-      <c r="E11">
+      <c r="E15" s="2">
         <v>-0.90904383536546407</v>
       </c>
-      <c r="F11">
+      <c r="F15" s="2">
         <v>-0.8627956639382367</v>
       </c>
-      <c r="G11" t="s">
+      <c r="G15" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="H11">
+      <c r="H15">
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="2:8" hidden="1" x14ac:dyDescent="0.35">
-      <c r="B12" t="s">
-        <v>5</v>
-      </c>
-      <c r="C12">
-        <v>-0.53246994822591609</v>
-      </c>
-      <c r="D12">
-        <v>-0.79359322745568095</v>
-      </c>
-      <c r="E12">
-        <v>-0.75392270877999112</v>
-      </c>
-      <c r="F12">
-        <v>-0.71018114887203065</v>
-      </c>
-      <c r="G12" t="s">
+    <row r="16" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B16" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" s="2">
+        <v>-0.45443687792318754</v>
+      </c>
+      <c r="D16" s="2">
+        <v>-0.62230641800395947</v>
+      </c>
+      <c r="E16" s="2">
+        <v>-0.87172115521818738</v>
+      </c>
+      <c r="F16" s="2">
+        <v>-0.75029799695316901</v>
+      </c>
+      <c r="G16" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="H12">
+      <c r="H16">
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B13" t="s">
+    <row r="17" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="B17" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C13">
-        <v>-0.45443687792318754</v>
-      </c>
-      <c r="D13">
-        <v>-0.62230641800395947</v>
-      </c>
-      <c r="E13">
-        <v>-0.87172115521818738</v>
-      </c>
-      <c r="F13">
-        <v>-0.75029799695316901</v>
-      </c>
-      <c r="G13" t="s">
-        <v>0</v>
-      </c>
-      <c r="H13">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="14" spans="2:8" hidden="1" x14ac:dyDescent="0.35">
-      <c r="B14" t="s">
-        <v>5</v>
-      </c>
-      <c r="C14">
-        <v>-0.19103890278885322</v>
-      </c>
-      <c r="D14">
-        <v>-1.5624617602267566E-2</v>
-      </c>
-      <c r="E14">
-        <v>-0.57593386729312046</v>
-      </c>
-      <c r="F14">
-        <v>-3.1345402429609481E-2</v>
-      </c>
-      <c r="G14" t="s">
-        <v>7</v>
-      </c>
-      <c r="H14">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="15" spans="2:8" hidden="1" x14ac:dyDescent="0.35">
-      <c r="B15" t="s">
-        <v>6</v>
-      </c>
-      <c r="C15">
-        <v>-0.4960459807218307</v>
-      </c>
-      <c r="D15">
-        <v>-0.54134520440419731</v>
-      </c>
-      <c r="E15">
-        <v>-0.78390812098357465</v>
-      </c>
-      <c r="F15">
-        <v>-0.75054705324224213</v>
-      </c>
-      <c r="G15" t="s">
-        <v>8</v>
-      </c>
-      <c r="H15">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="16" spans="2:8" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B16" t="s">
-        <v>5</v>
-      </c>
-      <c r="C16">
-        <v>-0.57230055083887155</v>
-      </c>
-      <c r="D16">
-        <v>-0.80095082363904357</v>
-      </c>
-      <c r="E16">
-        <v>-0.70901597017509299</v>
-      </c>
-      <c r="F16">
-        <v>-0.7387123142517128</v>
-      </c>
-      <c r="G16" t="s">
-        <v>0</v>
-      </c>
-      <c r="H16">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="17" spans="2:8" hidden="1" x14ac:dyDescent="0.35">
-      <c r="B17" t="s">
-        <v>6</v>
-      </c>
-      <c r="C17">
+      <c r="C17" s="2">
         <v>6.6543334560536793E-3</v>
       </c>
-      <c r="D17">
+      <c r="D17" s="2">
         <v>7.0987319974828253E-2</v>
       </c>
-      <c r="E17">
+      <c r="E17" s="2">
         <v>-0.57656548619946735</v>
       </c>
-      <c r="F17">
+      <c r="F17" s="2">
         <v>-0.1694141927084977</v>
       </c>
-      <c r="G17" t="s">
+      <c r="G17" s="4" t="s">
         <v>7</v>
       </c>
       <c r="H17">
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B18" t="s">
+    <row r="18" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="B18" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C18">
-        <v>-0.36116740939242498</v>
-      </c>
-      <c r="D18">
-        <v>-0.40347336681283164</v>
-      </c>
-      <c r="E18">
-        <v>-0.76011956622295818</v>
-      </c>
-      <c r="F18">
-        <v>-0.66626268288222079</v>
-      </c>
-      <c r="G18" t="s">
-        <v>0</v>
+      <c r="C18" s="2">
+        <v>-0.4960459807218307</v>
+      </c>
+      <c r="D18" s="2">
+        <v>-0.54134520440419731</v>
+      </c>
+      <c r="E18" s="2">
+        <v>-0.78390812098357465</v>
+      </c>
+      <c r="F18" s="2">
+        <v>-0.75054705324224213</v>
+      </c>
+      <c r="G18" s="4" t="s">
+        <v>8</v>
       </c>
       <c r="H18">
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="2:8" hidden="1" x14ac:dyDescent="0.35">
-      <c r="B19" t="s">
-        <v>5</v>
-      </c>
-      <c r="C19">
-        <v>-0.36902571311328258</v>
-      </c>
-      <c r="D19">
-        <v>0.15981874291995243</v>
-      </c>
-      <c r="E19">
-        <v>-0.19843610814515833</v>
-      </c>
-      <c r="F19">
-        <v>7.6033443732449343E-2</v>
-      </c>
-      <c r="G19" t="s">
-        <v>7</v>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="B19" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C19" s="2">
+        <v>-0.36116740939242498</v>
+      </c>
+      <c r="D19" s="2">
+        <v>-0.40347336681283164</v>
+      </c>
+      <c r="E19" s="2">
+        <v>-0.76011956622295818</v>
+      </c>
+      <c r="F19" s="2">
+        <v>-0.66626268288222079</v>
+      </c>
+      <c r="G19" s="4" t="s">
+        <v>0</v>
       </c>
       <c r="H19">
         <v>9</v>
       </c>
     </row>
-    <row r="20" spans="2:8" hidden="1" x14ac:dyDescent="0.35">
-      <c r="B20" t="s">
+    <row r="20" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="B20" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C20">
+      <c r="C20" s="2">
         <v>-9.9536103085989855E-2</v>
       </c>
-      <c r="D20">
+      <c r="D20" s="2">
         <v>0.33930944629576543</v>
       </c>
-      <c r="E20">
+      <c r="E20" s="2">
         <v>-0.16527367850382241</v>
       </c>
-      <c r="F20">
+      <c r="F20" s="2">
         <v>-7.6040969567188355E-3</v>
       </c>
-      <c r="G20" t="s">
+      <c r="G20" s="4" t="s">
         <v>7</v>
       </c>
       <c r="H20">

</xml_diff>